<commit_message>
4 tables added by Rakshanda
</commit_message>
<xml_diff>
--- a/Docs/Database Schema.xlsx
+++ b/Docs/Database Schema.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hites\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\Food-Catering\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAAED71-409B-4B12-8D51-30D30E120368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>Register &amp; Login</t>
   </si>
@@ -107,13 +106,52 @@
   </si>
   <si>
     <t>OID :- Order ID</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Review &amp; Rating</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Advertisment</t>
+  </si>
+  <si>
+    <t>Ad_ID</t>
+  </si>
+  <si>
+    <t>Serve_no</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>OID</t>
+  </si>
+  <si>
+    <t>Bill_no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -133,6 +171,21 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -142,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -150,16 +203,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,15 +448,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A18" sqref="A18:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -577,7 +651,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="6:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F17" s="3"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -585,18 +659,173 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="6:11" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="6:11" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="6:11" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="6:11" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="6:11" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="6:11" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="6:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="F30" s="2"/>
+    <row r="18" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes by Sir 14-08-2022
</commit_message>
<xml_diff>
--- a/Docs/Database Schema.xlsx
+++ b/Docs/Database Schema.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Desktop\CDAC-Project\Food-Catering\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229575D9-EBC0-4A63-8412-CA6A42C7FDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>Register &amp; Login</t>
   </si>
@@ -208,9 +202,6 @@
     <t>employee_picture_profile</t>
   </si>
   <si>
-    <t>employee_profile</t>
-  </si>
-  <si>
     <t>homemaker_tbl</t>
   </si>
   <si>
@@ -238,9 +229,6 @@
     <t>homemaker_picture_profile</t>
   </si>
   <si>
-    <t>homemaker_picture_post</t>
-  </si>
-  <si>
     <t>food_list_tbl</t>
   </si>
   <si>
@@ -256,27 +244,12 @@
     <t>food_category</t>
   </si>
   <si>
-    <t>payment_bill_no (pk)</t>
-  </si>
-  <si>
-    <t>payment_price</t>
-  </si>
-  <si>
     <t>consumer_id (fk)</t>
   </si>
   <si>
-    <t>homemaker_id</t>
-  </si>
-  <si>
     <t>food_id (fk)</t>
   </si>
   <si>
-    <t>address_details</t>
-  </si>
-  <si>
-    <t>payment_portal</t>
-  </si>
-  <si>
     <t>review_tbl</t>
   </si>
   <si>
@@ -286,18 +259,12 @@
     <t>food_rating</t>
   </si>
   <si>
-    <t>advertisement_tbl</t>
-  </si>
-  <si>
     <t>advertisement_id(pk)</t>
   </si>
   <si>
     <t>homemaker_id (fk)</t>
   </si>
   <si>
-    <t>advertisement_packages</t>
-  </si>
-  <si>
     <t>order_tbl</t>
   </si>
   <si>
@@ -310,29 +277,83 @@
     <t>consumer_id(fk)</t>
   </si>
   <si>
-    <t>payment_bill_no (fk)</t>
-  </si>
-  <si>
-    <t>location_tbl</t>
-  </si>
-  <si>
-    <t>location_pin</t>
-  </si>
-  <si>
-    <t>location_state</t>
-  </si>
-  <si>
-    <t>location__city</t>
-  </si>
-  <si>
     <t>Revised Data-Table</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>employee_role</t>
+  </si>
+  <si>
+    <t>qnt</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>food_image_tbl</t>
+  </si>
+  <si>
+    <t>image_id</t>
+  </si>
+  <si>
+    <t>image_data</t>
+  </si>
+  <si>
+    <t>food_id</t>
+  </si>
+  <si>
+    <t>image_name</t>
+  </si>
+  <si>
+    <t>post_tbl</t>
+  </si>
+  <si>
+    <t>total_qnt</t>
+  </si>
+  <si>
+    <t>valid_till_date</t>
+  </si>
+  <si>
+    <t>valid_till_time</t>
+  </si>
+  <si>
+    <t>total_amout</t>
+  </si>
+  <si>
+    <t>shipping_address</t>
+  </si>
+  <si>
+    <t>order_status</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>order_time</t>
+  </si>
+  <si>
+    <t>order_details_tbl</t>
+  </si>
+  <si>
+    <t>order_id (fk)</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>order_item_id</t>
+  </si>
+  <si>
+    <t>order_item_id (fk)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -417,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -440,11 +461,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -487,6 +519,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,18 +738,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z75"/>
+  <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
@@ -727,12 +764,12 @@
     <col min="11" max="11" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -758,17 +795,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.2">
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.2">
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.2">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -776,7 +813,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -795,14 +832,14 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.2">
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.2">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -811,7 +848,7 @@
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.2">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -824,7 +861,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -849,7 +886,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.2">
       <c r="F11" s="3"/>
       <c r="G11" s="1"/>
       <c r="J11" s="1" t="s">
@@ -857,14 +894,14 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.2">
       <c r="F12" s="3"/>
       <c r="G12" s="1"/>
       <c r="I12" s="3"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.2">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -874,7 +911,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.2">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -898,14 +935,14 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="13.2">
       <c r="F15" s="3"/>
       <c r="G15" s="1"/>
       <c r="I15" s="3"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.4" customHeight="1">
       <c r="F16" s="3"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -913,7 +950,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="13.8" thickBot="1">
       <c r="F17" s="3"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -921,7 +958,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="13.8" thickBot="1">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>22</v>
@@ -931,7 +968,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
@@ -947,7 +984,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -955,7 +992,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="13.8" thickBot="1">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -963,7 +1000,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="13.8" thickBot="1">
       <c r="A22" s="5"/>
       <c r="B22" s="6" t="s">
         <v>33</v>
@@ -973,7 +1010,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
@@ -989,7 +1026,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -997,7 +1034,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="13.8" thickBot="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1005,7 +1042,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="13.8" thickBot="1">
       <c r="A26" s="5"/>
       <c r="B26" s="6" t="s">
         <v>36</v>
@@ -1015,7 +1052,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
@@ -1031,7 +1068,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1039,7 +1076,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="13.8" thickBot="1">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1047,7 +1084,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="13.8" thickBot="1">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
         <v>39</v>
@@ -1057,7 +1094,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>40</v>
       </c>
@@ -1077,7 +1114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1085,13 +1122,13 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="E35" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>42</v>
@@ -1121,7 +1158,7 @@
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A39" s="9" t="s">
         <v>43</v>
       </c>
@@ -1149,12 +1186,13 @@
       <c r="I39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J39" s="11" t="s">
+      <c r="J39" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
@@ -1169,7 +1207,7 @@
       <c r="Y39" s="5"/>
       <c r="Z39" s="5"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="5"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
@@ -1197,7 +1235,7 @@
       <c r="Y40" s="5"/>
       <c r="Z40" s="5"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A41" s="5"/>
       <c r="B41" s="8" t="s">
         <v>53</v>
@@ -1227,7 +1265,7 @@
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
     </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A42" s="12" t="s">
         <v>54</v>
       </c>
@@ -1253,7 +1291,7 @@
         <v>61</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
@@ -1273,7 +1311,7 @@
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
     </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1301,10 +1339,10 @@
       <c r="Y43" s="5"/>
       <c r="Z43" s="5"/>
     </row>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A44" s="5"/>
       <c r="B44" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -1331,34 +1369,32 @@
       <c r="Y44" s="5"/>
       <c r="Z44" s="5"/>
     </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A45" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="C45" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="D45" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="E45" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="F45" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="G45" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="H45" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H45" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>72</v>
-      </c>
+      <c r="I45" s="13"/>
       <c r="J45" s="13" t="s">
         <v>51</v>
       </c>
@@ -1381,7 +1417,7 @@
       <c r="Y45" s="5"/>
       <c r="Z45" s="5"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1409,10 +1445,10 @@
       <c r="Y46" s="5"/>
       <c r="Z46" s="5"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A47" s="5"/>
       <c r="B47" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1439,22 +1475,28 @@
       <c r="Y47" s="5"/>
       <c r="Z47" s="5"/>
     </row>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A48" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="D48" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
+      <c r="E48" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
@@ -1475,7 +1517,7 @@
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
     </row>
-    <row r="49" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A49" s="5"/>
       <c r="B49" s="7"/>
       <c r="C49" s="5"/>
@@ -1503,8 +1545,27 @@
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
     </row>
-    <row r="51" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B50" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A51" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A52" s="5"/>
       <c r="B52" s="7"/>
       <c r="C52" s="5"/>
@@ -1513,143 +1574,122 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A53" s="5"/>
-      <c r="B53" s="7"/>
+      <c r="B53" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+    <row r="54" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A54" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F55" s="13" t="s">
+    <row r="55" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A56" s="5"/>
+      <c r="B56" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G55" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-    </row>
-    <row r="58" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A57" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A58" s="5"/>
-      <c r="B58" s="8" t="s">
-        <v>85</v>
-      </c>
+      <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-    </row>
-    <row r="62" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-    </row>
-    <row r="64" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B59" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A60" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="62" spans="1:26" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="63" spans="1:26" s="5" customFormat="1" ht="15.75" customHeight="1" thickBot="1"/>
+    <row r="64" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A64" s="5"/>
       <c r="B64" s="8" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -1657,24 +1697,24 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>90</v>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A65" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -1683,7 +1723,7 @@
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -1692,91 +1732,23 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
       <c r="A68" s="5"/>
-      <c r="B68" s="8" t="s">
-        <v>92</v>
-      </c>
+      <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="13" t="s">
-        <v>83</v>
-      </c>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
       <c r="G69" s="5"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="5"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="5"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="5"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="5"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="5"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>

</xml_diff>